<commit_message>
Les CSV og Skrifar PDF
Virkni komin, þarf að hanna ID betur og layout
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Skólinn\github\Isalp_felagaskyrteini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{84A607E3-F82F-4861-8A05-F02C12B74665}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7FC087-B23F-46F1-904C-815A02CE2296}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -20,39 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Nafn</t>
+    <t>Nafn,Aldur</t>
   </si>
   <si>
-    <t>Aldur</t>
+    <t>Jón,10</t>
   </si>
   <si>
-    <t>Jón</t>
+    <t>Gunnar,20</t>
   </si>
   <si>
-    <t>Alli</t>
+    <t>Alli,30</t>
   </si>
   <si>
-    <t>Hugrún</t>
+    <t>Hugrún,18</t>
   </si>
   <si>
-    <t>Nína</t>
+    <t>Nína,24</t>
   </si>
   <si>
-    <t>Albert</t>
+    <t>Albert,65</t>
   </si>
   <si>
-    <t>Lísa</t>
-  </si>
-  <si>
-    <t>Gunnar</t>
+    <t>Lísa,33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,77 +883,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>65</v>
-      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
-      </c>
-      <c r="B8">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>